<commit_message>
table of regression ols
</commit_message>
<xml_diff>
--- a/results/rmse_models.xlsx
+++ b/results/rmse_models.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\danie\Documents\GitHub\time_series_padova\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D5AECD2-9CE5-43B0-8B1B-96DD48A99B83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DF1A95E-D96A-4C66-B745-58A561D79EB8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{A633EDBC-9148-4D69-883F-A1C7AB227CFD}"/>
   </bookViews>
@@ -254,28 +254,19 @@
   <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="3" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="3" fontId="3" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="3" fontId="3" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="3" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="3" fontId="3" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -302,8 +293,17 @@
     <xf numFmtId="3" fontId="2" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="3" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2086,7 +2086,7 @@
   <dimension ref="B6:E15"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A5" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E25" sqref="E25"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -2098,136 +2098,136 @@
   </cols>
   <sheetData>
     <row r="6" spans="2:5">
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3"/>
-      <c r="E6" s="4"/>
+      <c r="C6" s="17"/>
+      <c r="D6" s="17"/>
+      <c r="E6" s="18"/>
     </row>
     <row r="7" spans="2:5">
-      <c r="B7" s="12" t="s">
+      <c r="B7" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="C7" s="5" t="s">
+      <c r="C7" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D7" s="5" t="s">
+      <c r="D7" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E7" s="6" t="s">
+      <c r="E7" s="3" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="8" spans="2:5">
-      <c r="B8" s="13" t="s">
+      <c r="B8" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="C8" s="7">
+      <c r="C8" s="4">
         <v>13229295</v>
       </c>
-      <c r="D8" s="7">
+      <c r="D8" s="4">
         <v>4000370</v>
       </c>
-      <c r="E8" s="8">
+      <c r="E8" s="5">
         <v>1421301</v>
       </c>
     </row>
     <row r="9" spans="2:5">
-      <c r="B9" s="14" t="s">
+      <c r="B9" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="C9" s="9">
+      <c r="C9" s="6">
         <v>18498870</v>
       </c>
-      <c r="D9" s="9">
+      <c r="D9" s="6">
         <v>4542019</v>
       </c>
-      <c r="E9" s="10">
+      <c r="E9" s="7">
         <v>1651896</v>
       </c>
     </row>
     <row r="10" spans="2:5">
-      <c r="B10" s="13" t="s">
+      <c r="B10" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="C10" s="18">
+      <c r="C10" s="15">
         <v>11759505</v>
       </c>
-      <c r="D10" s="7">
+      <c r="D10" s="4">
         <v>3453199</v>
       </c>
-      <c r="E10" s="8">
+      <c r="E10" s="5">
         <v>1600510</v>
       </c>
     </row>
     <row r="11" spans="2:5">
-      <c r="B11" s="14" t="s">
+      <c r="B11" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="C11" s="9">
+      <c r="C11" s="6">
         <v>13169921</v>
       </c>
-      <c r="D11" s="9" t="s">
+      <c r="D11" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="E11" s="10" t="s">
+      <c r="E11" s="7" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="12" spans="2:5">
-      <c r="B12" s="13" t="s">
+      <c r="B12" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="C12" s="7">
+      <c r="C12" s="4">
         <v>15118942</v>
       </c>
-      <c r="D12" s="7">
+      <c r="D12" s="4">
         <v>3328293</v>
       </c>
-      <c r="E12" s="8">
+      <c r="E12" s="5">
         <v>1094980</v>
       </c>
     </row>
     <row r="13" spans="2:5">
-      <c r="B13" s="13" t="s">
+      <c r="B13" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="C13" s="7">
+      <c r="C13" s="4">
         <v>16189623</v>
       </c>
-      <c r="D13" s="7">
+      <c r="D13" s="4">
         <v>3331847</v>
       </c>
-      <c r="E13" s="8">
+      <c r="E13" s="5">
         <v>1642520</v>
       </c>
     </row>
     <row r="14" spans="2:5">
-      <c r="B14" s="14" t="s">
+      <c r="B14" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="C14" s="9">
+      <c r="C14" s="6">
         <v>12123823</v>
       </c>
-      <c r="D14" s="9">
+      <c r="D14" s="6">
         <v>4027032</v>
       </c>
-      <c r="E14" s="10">
+      <c r="E14" s="7">
         <v>2053161</v>
       </c>
     </row>
     <row r="15" spans="2:5">
-      <c r="B15" s="15" t="s">
+      <c r="B15" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="C15" s="11">
+      <c r="C15" s="8">
         <v>16786939</v>
       </c>
-      <c r="D15" s="16">
+      <c r="D15" s="13">
         <v>3246088</v>
       </c>
-      <c r="E15" s="17">
+      <c r="E15" s="14">
         <v>1071375</v>
       </c>
     </row>

</xml_diff>